<commit_message>
Update requirements.txt with lightgbm
</commit_message>
<xml_diff>
--- a/backend/benchmarkTesting/content_analysis_results_20250707_000506.xlsx
+++ b/backend/benchmarkTesting/content_analysis_results_20250707_000506.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indsa\Downloads\internship\MARV_content_moderation_engine\backend\benchmarkTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919E9FE4-466E-4DCE-93FA-1FE1BFD33CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686252CD-33B8-4246-821C-CE1CC7320E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2746,11 +2746,12 @@
   <dimension ref="A1:P216"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="3" max="3" width="60.796875" customWidth="1"/>
     <col min="13" max="13" width="17.86328125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>